<commit_message>
Completed initial testing of CLI Preparation for vpls 2 remaining additions for Pre-log and design template checks
</commit_message>
<xml_diff>
--- a/Files_for_testing/Cli_prep_test_files/File_1.xlsx
+++ b/Files_for_testing/Cli_prep_test_files/File_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CLI_Automation\Files_for_testing\Cli_prep_test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F0DF20-DF40-4EE6-A1B4-FA22CDFEB1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF2C8C4-465C-432C-A83F-F3A9EDC00A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="172.31.72.93" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="64">
   <si>
     <t>VPLS-1#Secti0n_MPBN</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>A:Modify</t>
+  </si>
+  <si>
+    <t>VPLS Status</t>
+  </si>
+  <si>
+    <t>VSD Domain(Exist/New)</t>
   </si>
 </sst>
 </file>
@@ -708,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94300975-E9C6-46C2-B492-068F2C7BA8F5}">
-  <dimension ref="A1:BJ13"/>
+  <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+    <sheetView topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,7 +747,7 @@
     <col min="63" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -805,7 +811,7 @@
       <c r="BI1" s="1"/>
       <c r="BJ1" s="1"/>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -875,7 +881,7 @@
       <c r="BI2" s="1"/>
       <c r="BJ2" s="1"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -898,39 +904,41 @@
         <v>9</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -974,8 +982,9 @@
       <c r="BH3" s="1"/>
       <c r="BI3" s="1"/>
       <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:64" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -997,32 +1006,32 @@
       <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="11"/>
+      <c r="N4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="O4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="1"/>
+      <c r="S4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -1066,8 +1075,9 @@
       <c r="BH4" s="1"/>
       <c r="BI4" s="1"/>
       <c r="BJ4" s="1"/>
+      <c r="BK4" s="1"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:64" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -1089,30 +1099,30 @@
       <c r="G5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="12" t="s">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -1156,8 +1166,9 @@
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
       <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:64" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -1179,32 +1190,32 @@
       <c r="G6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="11"/>
+      <c r="N6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="1"/>
+      <c r="S6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -1248,8 +1259,9 @@
       <c r="BH6" s="1"/>
       <c r="BI6" s="1"/>
       <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:64" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -1271,30 +1283,30 @@
       <c r="G7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="11"/>
+      <c r="N7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="1"/>
+      <c r="S7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -1338,8 +1350,9 @@
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
       <c r="BJ7" s="1"/>
+      <c r="BK7" s="1"/>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -1403,7 +1416,7 @@
       <c r="BI8" s="1"/>
       <c r="BJ8" s="1"/>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="1"/>
@@ -1467,7 +1480,7 @@
       <c r="BI9" s="1"/>
       <c r="BJ9" s="1"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1547,7 +1560,7 @@
       <c r="BI10" s="1"/>
       <c r="BJ10" s="1"/>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -1561,52 +1574,56 @@
         <v>7</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="K11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="M11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="O11" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="P11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="Q11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="R11" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="S11" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="U11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -1648,8 +1665,10 @@
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
       <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
+      <c r="BL11" s="1"/>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="4"/>
@@ -1657,20 +1676,20 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="16"/>
+      <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="P12" s="16"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1712,8 +1731,10 @@
       <c r="BH12" s="1"/>
       <c r="BI12" s="1"/>
       <c r="BJ12" s="1"/>
+      <c r="BK12" s="1"/>
+      <c r="BL12" s="1"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="4"/>
@@ -1727,14 +1748,14 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="1"/>
+      <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="P13" s="1"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -1776,6 +1797,8 @@
       <c r="BH13" s="1"/>
       <c r="BI13" s="1"/>
       <c r="BJ13" s="1"/>
+      <c r="BK13" s="1"/>
+      <c r="BL13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1784,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA60B73C-386D-4108-BFDF-218B573190BC}">
-  <dimension ref="A1:BJ13"/>
+  <dimension ref="A1:BK13"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:R7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1817,7 +1840,7 @@
     <col min="63" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1881,7 +1904,7 @@
       <c r="BI1" s="1"/>
       <c r="BJ1" s="1"/>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1951,7 +1974,7 @@
       <c r="BI2" s="1"/>
       <c r="BJ2" s="1"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1974,39 +1997,41 @@
         <v>9</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -2050,8 +2075,9 @@
       <c r="BH3" s="1"/>
       <c r="BI3" s="1"/>
       <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2073,28 +2099,28 @@
       <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="1"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="12"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -2138,8 +2164,9 @@
       <c r="BH4" s="1"/>
       <c r="BI4" s="1"/>
       <c r="BJ4" s="1"/>
+      <c r="BK4" s="1"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2161,30 +2188,30 @@
       <c r="G5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="12"/>
-      <c r="S5" s="1"/>
+      <c r="S5" s="12"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -2228,8 +2255,9 @@
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
       <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2251,30 +2279,30 @@
       <c r="G6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="11"/>
+      <c r="N6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="12"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -2318,8 +2346,9 @@
       <c r="BH6" s="1"/>
       <c r="BI6" s="1"/>
       <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2341,28 +2370,28 @@
       <c r="G7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="M7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="11"/>
       <c r="N7" s="11"/>
-      <c r="O7" s="1"/>
+      <c r="O7" s="11"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="12"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -2406,8 +2435,9 @@
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
       <c r="BJ7" s="1"/>
+      <c r="BK7" s="1"/>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -2471,7 +2501,7 @@
       <c r="BI8" s="1"/>
       <c r="BJ8" s="1"/>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="1"/>
@@ -2535,7 +2565,7 @@
       <c r="BI9" s="1"/>
       <c r="BJ9" s="1"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -2615,7 +2645,7 @@
       <c r="BI10" s="1"/>
       <c r="BJ10" s="1"/>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -2650,30 +2680,32 @@
         <v>10</v>
       </c>
       <c r="L11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="N11" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="O11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="P11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="Q11" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="R11" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="S11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -2716,8 +2748,9 @@
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
       <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="4"/>
@@ -2731,13 +2764,13 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="16"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="1"/>
+      <c r="T12" s="4"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
@@ -2780,8 +2813,9 @@
       <c r="BH12" s="1"/>
       <c r="BI12" s="1"/>
       <c r="BJ12" s="1"/>
+      <c r="BK12" s="1"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="4"/>
@@ -2795,13 +2829,13 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="1"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="1"/>
+      <c r="T13" s="4"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -2844,6 +2878,7 @@
       <c r="BH13" s="1"/>
       <c r="BI13" s="1"/>
       <c r="BJ13" s="1"/>
+      <c r="BK13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>